<commit_message>
update water sampling logs
</commit_message>
<xml_diff>
--- a/pH_glider/water_sampling/sample_logs/RMI2_pH_Water_Sample_Deployment_Notes.xlsx
+++ b/pH_glider/water_sampling/sample_logs/RMI2_pH_Water_Sample_Deployment_Notes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/garzio/Documents/repo/rucool/dataset_archiving/pH_glider/water_sampling/sample_logs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33CE3FA7-0A3C-8146-BB55-A9822A2FCFF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9A2A0C9-8C84-4740-BECA-6C8707D7312F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="21860" windowHeight="21900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SampleLog" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
   <si>
     <t>Deployment Notes</t>
   </si>
@@ -68,6 +68,18 @@
   </si>
   <si>
     <t>Had issues with rosette. The bottom and thermocline (7, 14m) samples from the first cast were from the rosette, the rest of the samples captured with a single niskin. Temp/salinity are from the glider. People: Brian Buckingham, Jess Leonard, Delphine Mossman and Benjamin Lerner</t>
+  </si>
+  <si>
+    <t>RMI 2025 Spring Recovery</t>
+  </si>
+  <si>
+    <t>recovery</t>
+  </si>
+  <si>
+    <t>Collected extra deep samples, 4 bottles (2 pH, 2 TA) from 2 niskins per cast.
+Cast2 didn't close bottles, so redid cast
+Rosette didn't close 2m bottle on 3nd cast, so collected 2m sample immediately after rosette back on board for the 3nd profile samples.
+There is some issue with the ctd talking to the rosette, maybe a connection or cable issue? The bottle files had jumbled/weird characters, so couldn't process those files. Temp/Sal are from the CTD binned cnv files from the ctd on the rosette during the water collection. People: Nicole Waite, Brian Buckingham, Jess Leonard and Delphine Mossman</t>
   </si>
 </sst>
 </file>
@@ -419,7 +431,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -429,10 +441,10 @@
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="6.83203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.6640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="87" customWidth="1"/>
   </cols>
   <sheetData>
@@ -474,6 +486,26 @@
       </c>
       <c r="F2" s="3" t="s">
         <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="128" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" s="2">
+        <v>45797</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update pH water sampling
</commit_message>
<xml_diff>
--- a/pH_glider/water_sampling/sample_logs/RMI2_pH_Water_Sample_Deployment_Notes.xlsx
+++ b/pH_glider/water_sampling/sample_logs/RMI2_pH_Water_Sample_Deployment_Notes.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10727"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11116"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/garzio/Documents/repo/rucool/dataset_archiving/pH_glider/water_sampling/sample_logs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E78CC686-1798-4F42-9CE7-3315D700F6A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A2D58F8-04CA-CF48-90EA-AD34A72A4617}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-34860" yWindow="3020" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2580" yWindow="3400" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SampleLog" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="29">
   <si>
     <t>Deployment Notes</t>
   </si>
@@ -107,13 +107,28 @@
     <t>ru39-20250716T1542</t>
   </si>
   <si>
-    <t>Used CTD/rosette with no issues, People: Nicole, Lori, Dave, MOO students, Seatow vessel Jennie Lee.
-NOTE on the DEP glider ru32 that was deployed with ru39 - ru32 had issues and was recovered by Sea Tow without RU staff so there are no water samples for that glider recovery</t>
-  </si>
-  <si>
     <t>Took 2 water samples from the tank while the gliders (ru32 and ru39) were soaking. Ru39 log file: 0280.0000. ru32 log file: 0245.0000. People: Nicole Waite
 ru32: temp=23.206 cond=4.471, salinity=30.0658, pH_ref_voltage=-1.07314, pH=7.993031
 ru39: temp=23.204 cond=4.472, salinity=30.0746, pH_ref_voltage=-0.822675, pH=8.010643</t>
+  </si>
+  <si>
+    <t>RMI 2025 Fall Deployment</t>
+  </si>
+  <si>
+    <t>ru39-20251024T1506</t>
+  </si>
+  <si>
+    <t>RMI 2025 Fall Recovery</t>
+  </si>
+  <si>
+    <t>Used CTD/rosette with no issues, People: Nicole Waite, Lori Garzio, Dave Aragon, MOO students, Seatow vessel Jennie Lee.
+NOTE on the DEP glider ru32 that was deployed with ru39 - ru32 had issues and was recovered by Sea Tow without RU staff so there are no water samples for that glider recovery</t>
+  </si>
+  <si>
+    <t>Used single niskin to collect water samples at 2m and 8m. People: Brian Buckingham, Lori Garzio, Ashley Hann. Did the first cast, then went to remove tape from ru43 fluorometer, then continued with casts. Rough seas so we poisoned samples at the dock</t>
+  </si>
+  <si>
+    <t>Used rosette to collect water samples at 2m and 8m. For the first cast, the bottle for the 2m sample didn't close due to a mechanical issue, so immediately put the rosette back in the water to collect the surface sample. We consider this one cast since they were so close together. Very calm seas. People: Nicole Waite, Lori Garzio, Ashley Hann on the SeaTow Jennie Lee</t>
   </si>
 </sst>
 </file>
@@ -465,11 +480,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F12" sqref="F12"/>
+      <pane ySplit="1" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -556,7 +571,7 @@
         <v>45853</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="48" x14ac:dyDescent="0.2">
@@ -579,7 +594,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="48" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" ht="64" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -596,7 +611,47 @@
         <v>45880</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>22</v>
+        <v>26</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="48" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" t="s">
+        <v>23</v>
+      </c>
+      <c r="C7" t="s">
+        <v>24</v>
+      </c>
+      <c r="D7" t="s">
+        <v>9</v>
+      </c>
+      <c r="E7" s="2">
+        <v>45954</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="64" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8" t="s">
+        <v>25</v>
+      </c>
+      <c r="C8" t="s">
+        <v>24</v>
+      </c>
+      <c r="D8" t="s">
+        <v>12</v>
+      </c>
+      <c r="E8" s="2">
+        <v>45982</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>